<commit_message>
add assessment item to D, add rubric
</commit_message>
<xml_diff>
--- a/KnowledgeBase/sfia_v8_custom.xlsx
+++ b/KnowledgeBase/sfia_v8_custom.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\capstone\actual_project\accreditation_mapper_group_12_capstone_project\KnowledgeBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{671BE8DB-5EE8-47E0-8A1D-779F96414D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EEB52EA-1C61-4E63-81AA-45760B93AA33}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC2FCC9-361D-4CC5-8702-90B5C6C90887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{93CC7B8B-0745-4098-A127-811C5DAC2601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{93CC7B8B-0745-4098-A127-811C5DAC2601}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
@@ -3970,7 +3970,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4320,22 +4320,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A69E88-481B-476D-9126-0328EFC7F65C}">
   <dimension ref="A1:I496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="I175" sqref="I175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.26953125" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -5379,7 +5379,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>9</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>9</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>9</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>9</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>9</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -7235,7 +7235,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>9</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>9</v>
       </c>
@@ -7670,7 +7670,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -7757,7 +7757,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -7844,7 +7844,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -7989,7 +7989,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -8018,7 +8018,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -8076,7 +8076,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>9</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>9</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>9</v>
       </c>
@@ -8163,7 +8163,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>9</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>9</v>
       </c>
@@ -8221,7 +8221,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -8279,7 +8279,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -8308,7 +8308,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>9</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -8366,7 +8366,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -8453,7 +8453,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -8482,7 +8482,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -8511,7 +8511,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>9</v>
       </c>
@@ -8540,7 +8540,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>9</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>9</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>9</v>
       </c>
@@ -8685,7 +8685,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -8714,7 +8714,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -8743,7 +8743,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>9</v>
       </c>
@@ -8772,7 +8772,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>9</v>
       </c>
@@ -8801,7 +8801,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>9</v>
       </c>
@@ -8830,7 +8830,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>9</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -8888,7 +8888,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>9</v>
       </c>
@@ -8917,7 +8917,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -8946,7 +8946,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>9</v>
       </c>
@@ -8975,7 +8975,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>9</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>9</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>9</v>
       </c>
@@ -9062,7 +9062,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>9</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="45.75">
+    <row r="165" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>9</v>
       </c>
@@ -9120,7 +9120,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="60.75">
+    <row r="166" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>9</v>
       </c>
@@ -9149,7 +9149,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="60.75">
+    <row r="167" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -9178,7 +9178,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>9</v>
       </c>
@@ -9207,7 +9207,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>9</v>
       </c>
@@ -9236,7 +9236,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -9265,7 +9265,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>9</v>
       </c>
@@ -9294,7 +9294,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>9</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>9</v>
       </c>
@@ -9352,7 +9352,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>9</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>9</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>9</v>
       </c>
@@ -9439,7 +9439,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>9</v>
       </c>
@@ -9468,7 +9468,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>9</v>
       </c>
@@ -9497,7 +9497,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>9</v>
       </c>
@@ -9526,7 +9526,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>9</v>
       </c>
@@ -9555,7 +9555,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>9</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>9</v>
       </c>
@@ -9613,7 +9613,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>9</v>
       </c>
@@ -9642,7 +9642,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>9</v>
       </c>
@@ -9671,7 +9671,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>9</v>
       </c>
@@ -9700,7 +9700,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>9</v>
       </c>
@@ -9729,7 +9729,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>9</v>
       </c>
@@ -9758,7 +9758,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>9</v>
       </c>
@@ -9787,7 +9787,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>9</v>
       </c>
@@ -9816,7 +9816,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>9</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>9</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>9</v>
       </c>
@@ -9903,7 +9903,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>9</v>
       </c>
@@ -9932,7 +9932,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>9</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>9</v>
       </c>
@@ -9990,7 +9990,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>9</v>
       </c>
@@ -10019,7 +10019,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>9</v>
       </c>
@@ -10048,7 +10048,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>9</v>
       </c>
@@ -10077,7 +10077,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>9</v>
       </c>
@@ -10106,7 +10106,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>9</v>
       </c>
@@ -10135,7 +10135,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>9</v>
       </c>
@@ -10164,7 +10164,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>9</v>
       </c>
@@ -10193,7 +10193,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>9</v>
       </c>
@@ -10222,7 +10222,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>9</v>
       </c>
@@ -10251,7 +10251,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>9</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>9</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>9</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>9</v>
       </c>
@@ -10367,7 +10367,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="209" spans="1:9">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>9</v>
       </c>
@@ -10396,7 +10396,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="210" spans="1:9">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>9</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>9</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>9</v>
       </c>
@@ -10483,7 +10483,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>9</v>
       </c>
@@ -10512,7 +10512,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>9</v>
       </c>
@@ -10541,7 +10541,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>9</v>
       </c>
@@ -10570,7 +10570,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>9</v>
       </c>
@@ -10599,7 +10599,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>9</v>
       </c>
@@ -10628,7 +10628,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>9</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>9</v>
       </c>
@@ -10686,7 +10686,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>9</v>
       </c>
@@ -10715,7 +10715,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>9</v>
       </c>
@@ -10744,7 +10744,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>9</v>
       </c>
@@ -10773,7 +10773,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>9</v>
       </c>
@@ -10802,7 +10802,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>9</v>
       </c>
@@ -10831,7 +10831,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>9</v>
       </c>
@@ -10860,7 +10860,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>9</v>
       </c>
@@ -10889,7 +10889,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>9</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="228" spans="1:9">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>9</v>
       </c>
@@ -10947,7 +10947,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>9</v>
       </c>
@@ -10976,7 +10976,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="230" spans="1:9">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>9</v>
       </c>
@@ -11005,7 +11005,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="231" spans="1:9">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>9</v>
       </c>
@@ -11034,7 +11034,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>9</v>
       </c>
@@ -11063,7 +11063,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>9</v>
       </c>
@@ -11092,7 +11092,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="234" spans="1:9">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>9</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>9</v>
       </c>
@@ -11150,7 +11150,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>9</v>
       </c>
@@ -11179,7 +11179,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>9</v>
       </c>
@@ -11208,7 +11208,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>9</v>
       </c>
@@ -11237,7 +11237,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>9</v>
       </c>
@@ -11266,7 +11266,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>9</v>
       </c>
@@ -11295,7 +11295,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>9</v>
       </c>
@@ -11324,7 +11324,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>9</v>
       </c>
@@ -11353,7 +11353,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>9</v>
       </c>
@@ -11382,7 +11382,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>9</v>
       </c>
@@ -11411,7 +11411,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>9</v>
       </c>
@@ -11440,7 +11440,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>9</v>
       </c>
@@ -11469,7 +11469,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="247" spans="1:9">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>9</v>
       </c>
@@ -11498,7 +11498,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>9</v>
       </c>
@@ -11527,7 +11527,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>9</v>
       </c>
@@ -11556,7 +11556,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>9</v>
       </c>
@@ -11585,7 +11585,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>9</v>
       </c>
@@ -11614,7 +11614,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="252" spans="1:9">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>9</v>
       </c>
@@ -11643,7 +11643,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="253" spans="1:9">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>9</v>
       </c>
@@ -11672,7 +11672,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="254" spans="1:9">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>9</v>
       </c>
@@ -11701,7 +11701,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="255" spans="1:9">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>9</v>
       </c>
@@ -11730,7 +11730,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="256" spans="1:9">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>9</v>
       </c>
@@ -11759,7 +11759,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="257" spans="1:9">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>9</v>
       </c>
@@ -11788,7 +11788,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="258" spans="1:9">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>9</v>
       </c>
@@ -11817,7 +11817,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="259" spans="1:9">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>9</v>
       </c>
@@ -11846,7 +11846,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="260" spans="1:9">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>9</v>
       </c>
@@ -11875,7 +11875,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="261" spans="1:9">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>9</v>
       </c>
@@ -11904,7 +11904,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="262" spans="1:9">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>9</v>
       </c>
@@ -11933,7 +11933,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="263" spans="1:9">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>9</v>
       </c>
@@ -11962,7 +11962,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="264" spans="1:9">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>9</v>
       </c>
@@ -11991,7 +11991,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="265" spans="1:9">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>9</v>
       </c>
@@ -12020,7 +12020,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="266" spans="1:9">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>9</v>
       </c>
@@ -12049,7 +12049,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="267" spans="1:9">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>9</v>
       </c>
@@ -12078,7 +12078,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="268" spans="1:9">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>9</v>
       </c>
@@ -12107,7 +12107,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="269" spans="1:9">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>9</v>
       </c>
@@ -12136,7 +12136,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="270" spans="1:9">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>9</v>
       </c>
@@ -12165,7 +12165,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="271" spans="1:9">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>9</v>
       </c>
@@ -12194,7 +12194,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="272" spans="1:9">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>9</v>
       </c>
@@ -12223,7 +12223,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="273" spans="1:9">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>9</v>
       </c>
@@ -12252,7 +12252,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="274" spans="1:9">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>9</v>
       </c>
@@ -12281,7 +12281,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="275" spans="1:9">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>9</v>
       </c>
@@ -12310,7 +12310,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="276" spans="1:9">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>9</v>
       </c>
@@ -12339,7 +12339,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="277" spans="1:9">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>9</v>
       </c>
@@ -12368,7 +12368,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="278" spans="1:9">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>9</v>
       </c>
@@ -12397,7 +12397,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="279" spans="1:9">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>9</v>
       </c>
@@ -12426,7 +12426,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="280" spans="1:9">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>9</v>
       </c>
@@ -12455,7 +12455,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="281" spans="1:9">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>9</v>
       </c>
@@ -12484,7 +12484,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="282" spans="1:9">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>9</v>
       </c>
@@ -12513,7 +12513,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="283" spans="1:9">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>9</v>
       </c>
@@ -12542,7 +12542,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="284" spans="1:9">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>9</v>
       </c>
@@ -12571,7 +12571,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="285" spans="1:9">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>9</v>
       </c>
@@ -12600,7 +12600,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="286" spans="1:9">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>9</v>
       </c>
@@ -12629,7 +12629,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="287" spans="1:9">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>9</v>
       </c>
@@ -12658,7 +12658,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="288" spans="1:9">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>9</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="289" spans="1:9">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>9</v>
       </c>
@@ -12716,7 +12716,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="290" spans="1:9">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>9</v>
       </c>
@@ -12745,7 +12745,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="291" spans="1:9">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>9</v>
       </c>
@@ -12774,7 +12774,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="292" spans="1:9">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>9</v>
       </c>
@@ -12803,7 +12803,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="293" spans="1:9">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>9</v>
       </c>
@@ -12832,7 +12832,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="294" spans="1:9">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>9</v>
       </c>
@@ -12861,7 +12861,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="295" spans="1:9">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>9</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="296" spans="1:9">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>9</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="297" spans="1:9">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>9</v>
       </c>
@@ -12948,7 +12948,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="298" spans="1:9">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>9</v>
       </c>
@@ -12977,7 +12977,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="299" spans="1:9">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>9</v>
       </c>
@@ -13006,7 +13006,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="300" spans="1:9">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>9</v>
       </c>
@@ -13035,7 +13035,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="301" spans="1:9">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>9</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="302" spans="1:9">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>9</v>
       </c>
@@ -13093,7 +13093,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="303" spans="1:9">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>9</v>
       </c>
@@ -13122,7 +13122,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="304" spans="1:9">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>9</v>
       </c>
@@ -13151,7 +13151,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="305" spans="1:9">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>9</v>
       </c>
@@ -13180,7 +13180,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="306" spans="1:9">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>9</v>
       </c>
@@ -13209,7 +13209,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="307" spans="1:9">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>9</v>
       </c>
@@ -13238,7 +13238,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="308" spans="1:9">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>9</v>
       </c>
@@ -13267,7 +13267,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="309" spans="1:9">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>9</v>
       </c>
@@ -13296,7 +13296,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="310" spans="1:9">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>9</v>
       </c>
@@ -13325,7 +13325,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="311" spans="1:9">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>9</v>
       </c>
@@ -13354,7 +13354,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="312" spans="1:9">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>9</v>
       </c>
@@ -13383,7 +13383,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="313" spans="1:9">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>9</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="314" spans="1:9">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>9</v>
       </c>
@@ -13441,7 +13441,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="315" spans="1:9">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>9</v>
       </c>
@@ -13470,7 +13470,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="316" spans="1:9">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>9</v>
       </c>
@@ -13499,7 +13499,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="317" spans="1:9">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>9</v>
       </c>
@@ -13528,7 +13528,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="318" spans="1:9">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>9</v>
       </c>
@@ -13557,7 +13557,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="319" spans="1:9">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>9</v>
       </c>
@@ -13586,7 +13586,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="320" spans="1:9">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>9</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="321" spans="1:9">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>9</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="322" spans="1:9">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>9</v>
       </c>
@@ -13673,7 +13673,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="323" spans="1:9">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>9</v>
       </c>
@@ -13702,7 +13702,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="324" spans="1:9">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>9</v>
       </c>
@@ -13731,7 +13731,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="325" spans="1:9">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>9</v>
       </c>
@@ -13760,7 +13760,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="326" spans="1:9">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>9</v>
       </c>
@@ -13789,7 +13789,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="327" spans="1:9">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>9</v>
       </c>
@@ -13818,7 +13818,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="328" spans="1:9">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>9</v>
       </c>
@@ -13847,7 +13847,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="329" spans="1:9">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>9</v>
       </c>
@@ -13876,7 +13876,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>9</v>
       </c>
@@ -13905,7 +13905,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="331" spans="1:9">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>9</v>
       </c>
@@ -13934,7 +13934,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="332" spans="1:9">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>9</v>
       </c>
@@ -13963,7 +13963,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="333" spans="1:9">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>9</v>
       </c>
@@ -13992,7 +13992,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="334" spans="1:9">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>9</v>
       </c>
@@ -14021,7 +14021,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="335" spans="1:9">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>9</v>
       </c>
@@ -14050,7 +14050,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="336" spans="1:9">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>9</v>
       </c>
@@ -14079,7 +14079,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="337" spans="1:9">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>9</v>
       </c>
@@ -14108,7 +14108,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="338" spans="1:9">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>9</v>
       </c>
@@ -14137,7 +14137,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="339" spans="1:9">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>9</v>
       </c>
@@ -14166,7 +14166,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="340" spans="1:9">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>9</v>
       </c>
@@ -14195,7 +14195,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="341" spans="1:9">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>9</v>
       </c>
@@ -14224,7 +14224,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="342" spans="1:9">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>9</v>
       </c>
@@ -14253,7 +14253,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="343" spans="1:9">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>9</v>
       </c>
@@ -14282,7 +14282,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="344" spans="1:9">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>9</v>
       </c>
@@ -14311,7 +14311,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="345" spans="1:9">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>9</v>
       </c>
@@ -14340,7 +14340,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="346" spans="1:9">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>9</v>
       </c>
@@ -14369,7 +14369,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="347" spans="1:9">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>9</v>
       </c>
@@ -14398,7 +14398,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="348" spans="1:9">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>9</v>
       </c>
@@ -14427,7 +14427,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="349" spans="1:9">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>9</v>
       </c>
@@ -14456,7 +14456,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="350" spans="1:9">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>9</v>
       </c>
@@ -14485,7 +14485,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="351" spans="1:9">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>9</v>
       </c>
@@ -14514,7 +14514,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="352" spans="1:9">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>9</v>
       </c>
@@ -14543,7 +14543,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="353" spans="1:9">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>9</v>
       </c>
@@ -14572,7 +14572,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="354" spans="1:9">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>9</v>
       </c>
@@ -14601,7 +14601,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="355" spans="1:9">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>9</v>
       </c>
@@ -14630,7 +14630,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="356" spans="1:9">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>9</v>
       </c>
@@ -14659,7 +14659,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="357" spans="1:9">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>9</v>
       </c>
@@ -14688,7 +14688,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="358" spans="1:9">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>9</v>
       </c>
@@ -14717,7 +14717,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="359" spans="1:9">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>9</v>
       </c>
@@ -14746,7 +14746,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="360" spans="1:9">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>9</v>
       </c>
@@ -14775,7 +14775,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="361" spans="1:9">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>9</v>
       </c>
@@ -14804,7 +14804,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="362" spans="1:9">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>9</v>
       </c>
@@ -14833,7 +14833,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="363" spans="1:9">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>9</v>
       </c>
@@ -14862,7 +14862,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="364" spans="1:9">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>9</v>
       </c>
@@ -14891,7 +14891,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="365" spans="1:9">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>9</v>
       </c>
@@ -14920,7 +14920,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="366" spans="1:9">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>9</v>
       </c>
@@ -14949,7 +14949,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="367" spans="1:9">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>9</v>
       </c>
@@ -14978,7 +14978,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="368" spans="1:9">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>9</v>
       </c>
@@ -15007,7 +15007,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="369" spans="1:9">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>9</v>
       </c>
@@ -15036,7 +15036,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="370" spans="1:9">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
         <v>9</v>
       </c>
@@ -15065,7 +15065,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="371" spans="1:9">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
         <v>9</v>
       </c>
@@ -15094,7 +15094,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="372" spans="1:9">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
         <v>9</v>
       </c>
@@ -15123,7 +15123,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="373" spans="1:9">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
         <v>9</v>
       </c>
@@ -15152,7 +15152,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="374" spans="1:9">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
         <v>9</v>
       </c>
@@ -15181,7 +15181,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="375" spans="1:9">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
         <v>9</v>
       </c>
@@ -15210,7 +15210,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="376" spans="1:9">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
         <v>9</v>
       </c>
@@ -15239,7 +15239,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="377" spans="1:9">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
         <v>9</v>
       </c>
@@ -15268,7 +15268,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="378" spans="1:9">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
         <v>9</v>
       </c>
@@ -15297,7 +15297,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="379" spans="1:9">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
         <v>9</v>
       </c>
@@ -15326,7 +15326,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="380" spans="1:9">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
         <v>9</v>
       </c>
@@ -15355,7 +15355,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="381" spans="1:9">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
         <v>9</v>
       </c>
@@ -15384,7 +15384,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="382" spans="1:9">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
         <v>9</v>
       </c>
@@ -15413,7 +15413,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="383" spans="1:9">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
         <v>9</v>
       </c>
@@ -15442,7 +15442,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="384" spans="1:9">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
         <v>9</v>
       </c>
@@ -15471,7 +15471,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="385" spans="1:9">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
         <v>9</v>
       </c>
@@ -15500,7 +15500,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="386" spans="1:9">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
         <v>9</v>
       </c>
@@ -15529,7 +15529,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="387" spans="1:9">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
         <v>9</v>
       </c>
@@ -15558,7 +15558,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="388" spans="1:9">
+    <row r="388" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
         <v>9</v>
       </c>
@@ -15587,7 +15587,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="389" spans="1:9">
+    <row r="389" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
         <v>9</v>
       </c>
@@ -15616,7 +15616,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="390" spans="1:9">
+    <row r="390" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
         <v>9</v>
       </c>
@@ -15645,7 +15645,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="391" spans="1:9">
+    <row r="391" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
         <v>9</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="392" spans="1:9">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
         <v>9</v>
       </c>
@@ -15703,7 +15703,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="393" spans="1:9">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
         <v>9</v>
       </c>
@@ -15732,7 +15732,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="394" spans="1:9">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
         <v>9</v>
       </c>
@@ -15761,7 +15761,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="395" spans="1:9">
+    <row r="395" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
         <v>9</v>
       </c>
@@ -15790,7 +15790,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="396" spans="1:9">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
         <v>9</v>
       </c>
@@ -15819,7 +15819,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="397" spans="1:9">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
         <v>9</v>
       </c>
@@ -15848,7 +15848,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="398" spans="1:9">
+    <row r="398" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
         <v>9</v>
       </c>
@@ -15877,7 +15877,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="399" spans="1:9">
+    <row r="399" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
         <v>9</v>
       </c>
@@ -15906,7 +15906,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="400" spans="1:9">
+    <row r="400" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
         <v>9</v>
       </c>
@@ -15935,7 +15935,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="401" spans="1:9">
+    <row r="401" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
         <v>9</v>
       </c>
@@ -15964,7 +15964,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="402" spans="1:9">
+    <row r="402" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
         <v>9</v>
       </c>
@@ -15993,7 +15993,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="403" spans="1:9">
+    <row r="403" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
         <v>9</v>
       </c>
@@ -16022,7 +16022,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="404" spans="1:9">
+    <row r="404" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
         <v>9</v>
       </c>
@@ -16051,7 +16051,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="405" spans="1:9">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
         <v>9</v>
       </c>
@@ -16080,7 +16080,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="406" spans="1:9">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
         <v>9</v>
       </c>
@@ -16109,7 +16109,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="407" spans="1:9">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
         <v>9</v>
       </c>
@@ -16138,7 +16138,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="408" spans="1:9">
+    <row r="408" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
         <v>9</v>
       </c>
@@ -16167,7 +16167,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="409" spans="1:9">
+    <row r="409" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
         <v>9</v>
       </c>
@@ -16196,7 +16196,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="410" spans="1:9">
+    <row r="410" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
         <v>9</v>
       </c>
@@ -16225,7 +16225,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="411" spans="1:9">
+    <row r="411" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
         <v>9</v>
       </c>
@@ -16254,7 +16254,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="412" spans="1:9">
+    <row r="412" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
         <v>9</v>
       </c>
@@ -16283,7 +16283,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="413" spans="1:9">
+    <row r="413" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
         <v>9</v>
       </c>
@@ -16312,7 +16312,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="414" spans="1:9">
+    <row r="414" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
         <v>9</v>
       </c>
@@ -16341,7 +16341,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="415" spans="1:9">
+    <row r="415" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
         <v>9</v>
       </c>
@@ -16370,7 +16370,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="416" spans="1:9">
+    <row r="416" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
         <v>9</v>
       </c>
@@ -16399,7 +16399,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="417" spans="1:9">
+    <row r="417" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
         <v>9</v>
       </c>
@@ -16428,7 +16428,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="418" spans="1:9">
+    <row r="418" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
         <v>9</v>
       </c>
@@ -16457,7 +16457,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="419" spans="1:9">
+    <row r="419" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
         <v>9</v>
       </c>
@@ -16486,7 +16486,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="420" spans="1:9">
+    <row r="420" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
         <v>9</v>
       </c>
@@ -16515,7 +16515,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="421" spans="1:9">
+    <row r="421" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
         <v>9</v>
       </c>
@@ -16544,7 +16544,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="422" spans="1:9">
+    <row r="422" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
         <v>9</v>
       </c>
@@ -16573,7 +16573,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="423" spans="1:9">
+    <row r="423" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
         <v>9</v>
       </c>
@@ -16602,7 +16602,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="424" spans="1:9">
+    <row r="424" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
         <v>9</v>
       </c>
@@ -16631,7 +16631,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="425" spans="1:9">
+    <row r="425" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
         <v>9</v>
       </c>
@@ -16660,7 +16660,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="426" spans="1:9">
+    <row r="426" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
         <v>9</v>
       </c>
@@ -16689,7 +16689,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="427" spans="1:9">
+    <row r="427" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
         <v>9</v>
       </c>
@@ -16718,7 +16718,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="428" spans="1:9">
+    <row r="428" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
         <v>9</v>
       </c>
@@ -16747,7 +16747,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="429" spans="1:9">
+    <row r="429" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
         <v>9</v>
       </c>
@@ -16776,7 +16776,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="430" spans="1:9">
+    <row r="430" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
         <v>9</v>
       </c>
@@ -16805,7 +16805,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="431" spans="1:9">
+    <row r="431" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
         <v>9</v>
       </c>
@@ -16834,7 +16834,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="432" spans="1:9">
+    <row r="432" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
         <v>9</v>
       </c>
@@ -16863,7 +16863,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="433" spans="1:9">
+    <row r="433" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
         <v>9</v>
       </c>
@@ -16892,7 +16892,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="434" spans="1:9">
+    <row r="434" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
         <v>9</v>
       </c>
@@ -16921,7 +16921,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="435" spans="1:9">
+    <row r="435" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
         <v>9</v>
       </c>
@@ -16950,7 +16950,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="436" spans="1:9">
+    <row r="436" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
         <v>9</v>
       </c>
@@ -16979,7 +16979,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="437" spans="1:9">
+    <row r="437" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
         <v>9</v>
       </c>
@@ -17008,7 +17008,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="438" spans="1:9">
+    <row r="438" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
         <v>9</v>
       </c>
@@ -17037,7 +17037,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="439" spans="1:9">
+    <row r="439" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
         <v>9</v>
       </c>
@@ -17066,7 +17066,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="440" spans="1:9">
+    <row r="440" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
         <v>9</v>
       </c>
@@ -17095,7 +17095,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="441" spans="1:9">
+    <row r="441" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
         <v>9</v>
       </c>
@@ -17124,7 +17124,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="442" spans="1:9">
+    <row r="442" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
         <v>9</v>
       </c>
@@ -17153,7 +17153,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="443" spans="1:9">
+    <row r="443" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
         <v>9</v>
       </c>
@@ -17182,7 +17182,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="444" spans="1:9">
+    <row r="444" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
         <v>9</v>
       </c>
@@ -17211,7 +17211,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="445" spans="1:9">
+    <row r="445" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
         <v>9</v>
       </c>
@@ -17240,7 +17240,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="446" spans="1:9">
+    <row r="446" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
         <v>9</v>
       </c>
@@ -17269,7 +17269,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="447" spans="1:9">
+    <row r="447" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
         <v>9</v>
       </c>
@@ -17298,7 +17298,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="448" spans="1:9">
+    <row r="448" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
         <v>9</v>
       </c>
@@ -17327,7 +17327,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="449" spans="1:9">
+    <row r="449" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
         <v>9</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="450" spans="1:9">
+    <row r="450" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
         <v>9</v>
       </c>
@@ -17385,7 +17385,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="451" spans="1:9">
+    <row r="451" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
         <v>9</v>
       </c>
@@ -17414,7 +17414,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="452" spans="1:9">
+    <row r="452" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
         <v>9</v>
       </c>
@@ -17443,7 +17443,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="453" spans="1:9">
+    <row r="453" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
         <v>9</v>
       </c>
@@ -17472,7 +17472,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="454" spans="1:9">
+    <row r="454" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
         <v>9</v>
       </c>
@@ -17501,7 +17501,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="455" spans="1:9">
+    <row r="455" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
         <v>9</v>
       </c>
@@ -17530,7 +17530,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="456" spans="1:9">
+    <row r="456" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
         <v>9</v>
       </c>
@@ -17559,7 +17559,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="457" spans="1:9">
+    <row r="457" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
         <v>9</v>
       </c>
@@ -17588,7 +17588,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="458" spans="1:9">
+    <row r="458" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
         <v>9</v>
       </c>
@@ -17617,7 +17617,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="459" spans="1:9">
+    <row r="459" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
         <v>9</v>
       </c>
@@ -17646,7 +17646,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="460" spans="1:9">
+    <row r="460" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
         <v>9</v>
       </c>
@@ -17675,7 +17675,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="461" spans="1:9">
+    <row r="461" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
         <v>9</v>
       </c>
@@ -17704,7 +17704,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="462" spans="1:9">
+    <row r="462" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
         <v>9</v>
       </c>
@@ -17733,7 +17733,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="463" spans="1:9">
+    <row r="463" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
         <v>9</v>
       </c>
@@ -17762,7 +17762,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="464" spans="1:9">
+    <row r="464" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
         <v>9</v>
       </c>
@@ -17791,7 +17791,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="465" spans="1:9">
+    <row r="465" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
         <v>9</v>
       </c>
@@ -17820,7 +17820,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="466" spans="1:9">
+    <row r="466" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
         <v>9</v>
       </c>
@@ -17849,7 +17849,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="467" spans="1:9">
+    <row r="467" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
         <v>9</v>
       </c>
@@ -17878,7 +17878,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="468" spans="1:9">
+    <row r="468" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
         <v>9</v>
       </c>
@@ -17907,7 +17907,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="469" spans="1:9">
+    <row r="469" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
         <v>9</v>
       </c>
@@ -17936,7 +17936,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="470" spans="1:9">
+    <row r="470" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
         <v>9</v>
       </c>
@@ -17965,7 +17965,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="471" spans="1:9">
+    <row r="471" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
         <v>9</v>
       </c>
@@ -17994,7 +17994,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="472" spans="1:9">
+    <row r="472" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
         <v>9</v>
       </c>
@@ -18023,7 +18023,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="473" spans="1:9">
+    <row r="473" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
         <v>9</v>
       </c>
@@ -18052,7 +18052,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="474" spans="1:9">
+    <row r="474" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
         <v>9</v>
       </c>
@@ -18081,7 +18081,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="475" spans="1:9">
+    <row r="475" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
         <v>9</v>
       </c>
@@ -18110,7 +18110,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="476" spans="1:9">
+    <row r="476" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
         <v>9</v>
       </c>
@@ -18139,7 +18139,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="477" spans="1:9">
+    <row r="477" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
         <v>9</v>
       </c>
@@ -18168,7 +18168,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="478" spans="1:9">
+    <row r="478" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
         <v>9</v>
       </c>
@@ -18197,7 +18197,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="479" spans="1:9">
+    <row r="479" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
         <v>9</v>
       </c>
@@ -18226,7 +18226,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="480" spans="1:9">
+    <row r="480" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
         <v>9</v>
       </c>
@@ -18255,7 +18255,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="481" spans="1:9">
+    <row r="481" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
         <v>9</v>
       </c>
@@ -18284,7 +18284,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="482" spans="1:9">
+    <row r="482" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
         <v>9</v>
       </c>
@@ -18313,7 +18313,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="483" spans="1:9">
+    <row r="483" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
         <v>9</v>
       </c>
@@ -18342,7 +18342,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="484" spans="1:9">
+    <row r="484" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
         <v>9</v>
       </c>
@@ -18371,7 +18371,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="485" spans="1:9">
+    <row r="485" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
         <v>9</v>
       </c>
@@ -18400,7 +18400,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="486" spans="1:9">
+    <row r="486" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
         <v>9</v>
       </c>
@@ -18429,7 +18429,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="487" spans="1:9">
+    <row r="487" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
         <v>9</v>
       </c>
@@ -18458,7 +18458,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="488" spans="1:9">
+    <row r="488" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
         <v>9</v>
       </c>
@@ -18487,7 +18487,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="489" spans="1:9">
+    <row r="489" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
         <v>9</v>
       </c>
@@ -18516,7 +18516,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="490" spans="1:9">
+    <row r="490" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
         <v>9</v>
       </c>
@@ -18545,7 +18545,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="491" spans="1:9">
+    <row r="491" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
         <v>9</v>
       </c>
@@ -18574,7 +18574,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="492" spans="1:9">
+    <row r="492" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
         <v>9</v>
       </c>
@@ -18603,7 +18603,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="493" spans="1:9">
+    <row r="493" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
         <v>9</v>
       </c>
@@ -18632,7 +18632,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="494" spans="1:9">
+    <row r="494" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
         <v>9</v>
       </c>
@@ -18661,7 +18661,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="495" spans="1:9">
+    <row r="495" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
         <v>9</v>
       </c>
@@ -18690,7 +18690,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="496" spans="1:9">
+    <row r="496" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
         <v>9</v>
       </c>

</xml_diff>